<commit_message>
printStart, width and height passed
</commit_message>
<xml_diff>
--- a/cuentas.xlsx
+++ b/cuentas.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="ControllerUnit">Hoja1!$D$26</definedName>
     <definedName name="LaserDelay">Hoja1!$D$5</definedName>
     <definedName name="MaxLaserFrecuency">Hoja1!$D$13</definedName>
     <definedName name="MinimunPrintWidth">Hoja1!$D$16</definedName>
@@ -27,8 +28,11 @@
     <definedName name="PrinterWidth">Hoja1!$D$3</definedName>
     <definedName name="PWMFrecuency">Hoja1!$D$22</definedName>
     <definedName name="PWMResolution">Hoja1!$D$23</definedName>
+    <definedName name="RatioConvert">Hoja1!$C$27</definedName>
     <definedName name="Resolution">Hoja1!$D$4</definedName>
     <definedName name="ResolutionTime">Hoja1!$D$17</definedName>
+    <definedName name="Trailing">Hoja1!$D$9</definedName>
+    <definedName name="UnitInMicroMeters">Hoja1!$D$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Resolution</t>
   </si>
@@ -124,12 +128,33 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Trailing</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>UnitInMicroMeters</t>
+  </si>
+  <si>
+    <t>Controller Unit</t>
+  </si>
+  <si>
+    <t>Ratio Convert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -191,7 +216,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -474,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,14 +517,14 @@
     <col min="2" max="2" width="26.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="10" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1"/>
     <col min="7" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11.42578125" style="2"/>
     <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -517,7 +548,9 @@
       <c r="D3" s="1">
         <v>200000</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -529,7 +562,7 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -565,12 +598,39 @@
       <c r="D7" s="8">
         <v>45</v>
       </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="10">
+        <v>25400</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="10">
+        <v>5</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,7 +644,7 @@
       <c r="A12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
@@ -609,6 +669,9 @@
         <f>1/MotorSpeed*60*10^6</f>
         <v>24000</v>
       </c>
+      <c r="E14" s="10">
+        <v>2</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -619,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1">
-        <f>PrinterAngle/360*D14</f>
+        <f>PrinterAngle/360*MotorRevolution</f>
         <v>3000</v>
       </c>
     </row>
@@ -690,7 +753,6 @@
       <c r="D22" s="8">
         <v>144</v>
       </c>
-      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
@@ -717,7 +779,6 @@
         <f>LaserDelay*PWMFrecuency</f>
         <v>144</v>
       </c>
-      <c r="E24" s="8"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,6 +792,72 @@
         <f>MotorRevolution*PWMFrecuency</f>
         <v>3456000</v>
       </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1">
+        <f>1/(PWMFrecuency*10^6)*10^12</f>
+        <v>6944.4444444444443</v>
+      </c>
+      <c r="E26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1">
+        <f>(UnitInMicroMeters/10^Trailing)*(PrinterTimeLine/PrinterWidth)/(ControllerUnit*10^-6)</f>
+        <v>0.54864000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Signal revolution reception emulated on timer 3 channel 1, captured on timer 2 channel 2 and regenerated on channel 1
</commit_message>
<xml_diff>
--- a/cuentas.xlsx
+++ b/cuentas.xlsx
@@ -13,26 +13,28 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ControllerUnit">Hoja1!$D$26</definedName>
+    <definedName name="ControllerUnit">Hoja1!$D$27</definedName>
     <definedName name="LaserDelay">Hoja1!$D$5</definedName>
-    <definedName name="MaxLaserFrecuency">Hoja1!$D$13</definedName>
-    <definedName name="MinimunPrintWidth">Hoja1!$D$16</definedName>
-    <definedName name="MinimunPWMfrecuency">Hoja1!$D$18</definedName>
-    <definedName name="MinimunPWMresolution">Hoja1!$D$19</definedName>
-    <definedName name="MotorRevolution">Hoja1!$D$14</definedName>
-    <definedName name="MotorSpeed">Hoja1!$D$6</definedName>
-    <definedName name="PrinterAngle">Hoja1!$D$7</definedName>
-    <definedName name="PrinterTimeLine">Hoja1!$D$15</definedName>
+    <definedName name="MaxLaserFrecuency">Hoja1!$D$14</definedName>
+    <definedName name="MinimunPrintWidth">Hoja1!$D$17</definedName>
+    <definedName name="MinimunPWMfrecuency">Hoja1!$D$19</definedName>
+    <definedName name="MinimunPWMresolution">Hoja1!$D$20</definedName>
+    <definedName name="Mirrors">Hoja1!$D$6</definedName>
+    <definedName name="MotorRevolution">Hoja1!$D$15</definedName>
+    <definedName name="MotorSpeed">Hoja1!$D$7</definedName>
+    <definedName name="PrinterAngle">Hoja1!$D$8</definedName>
+    <definedName name="PrinterTimeLine">Hoja1!$D$16</definedName>
     <definedName name="PrinterWidth">Hoja1!$D$3</definedName>
-    <definedName name="PWMFrecuency">Hoja1!$D$22</definedName>
-    <definedName name="PWMResolution">Hoja1!$D$23</definedName>
-    <definedName name="RatioConvert">Hoja1!$C$27</definedName>
+    <definedName name="PWMFrecuency">Hoja1!$D$23</definedName>
+    <definedName name="PWMResolution">Hoja1!$D$24</definedName>
+    <definedName name="RatioConvert">Hoja1!$C$28</definedName>
     <definedName name="Resolution">Hoja1!$D$4</definedName>
-    <definedName name="ResolutionTime">Hoja1!$D$17</definedName>
-    <definedName name="Trailing">Hoja1!$D$9</definedName>
-    <definedName name="UnitInMicroMeters">Hoja1!$D$8</definedName>
+    <definedName name="ResolutionTime">Hoja1!$D$18</definedName>
+    <definedName name="Trailing">Hoja1!$D$10</definedName>
+    <definedName name="UnitInMicroMeters">Hoja1!$D$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Resolution</t>
   </si>
@@ -146,6 +148,72 @@
   </si>
   <si>
     <t>Ratio Convert</t>
+  </si>
+  <si>
+    <t>capture[0]</t>
+  </si>
+  <si>
+    <t>volatile uint16_t</t>
+  </si>
+  <si>
+    <t>capture[1]</t>
+  </si>
+  <si>
+    <t>capture[2]</t>
+  </si>
+  <si>
+    <t>capture[3]</t>
+  </si>
+  <si>
+    <t>capture[4]</t>
+  </si>
+  <si>
+    <t>capture[5]</t>
+  </si>
+  <si>
+    <t>capture[6]</t>
+  </si>
+  <si>
+    <t>capture[7]</t>
+  </si>
+  <si>
+    <t>capture[8]</t>
+  </si>
+  <si>
+    <t>capture[9]</t>
+  </si>
+  <si>
+    <t>capture[10]</t>
+  </si>
+  <si>
+    <t>capture[11]</t>
+  </si>
+  <si>
+    <t>capture[12]</t>
+  </si>
+  <si>
+    <t>capture[13]</t>
+  </si>
+  <si>
+    <t>capture[14]</t>
+  </si>
+  <si>
+    <t>capture[15]</t>
+  </si>
+  <si>
+    <t>capture[16]</t>
+  </si>
+  <si>
+    <t>capture[17]</t>
+  </si>
+  <si>
+    <t>capture[18]</t>
+  </si>
+  <si>
+    <t>capture[19]</t>
+  </si>
+  <si>
+    <t>Mirrors</t>
   </si>
 </sst>
 </file>
@@ -184,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -224,6 +292,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +589,7 @@
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="12.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11.42578125" style="2"/>
     <col min="11" max="16384" width="11.42578125" style="3"/>
@@ -578,55 +649,55 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D6" s="8">
-        <v>2500</v>
+        <v>2</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8">
-        <v>45</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1</v>
+        <v>2500</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="10">
-        <v>25400</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="8">
+        <v>45</v>
       </c>
       <c r="E8" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D9" s="10">
-        <v>5</v>
+        <v>25400</v>
       </c>
       <c r="E9" s="10">
         <v>2</v>
@@ -634,233 +705,561 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="8"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <f>1/LaserDelay</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <f>1/MotorSpeed*60*10^6</f>
         <v>24000</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E15" s="10">
         <v>2</v>
       </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f>PrinterAngle/360*MotorRevolution</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <f>LaserDelay*PrinterWidth/PrinterTimeLine</f>
         <v>66.666666666666671</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="1">
-        <f>Resolution*LaserDelay/D16</f>
+      <c r="D18" s="1">
+        <f>Resolution*LaserDelay/MinimunPrintWidth</f>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D19" s="10">
         <f>1/(Resolution*PrinterTimeLine/PrinterWidth)</f>
         <v>66.666666666666671</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8">
-        <f>ROUNDUP(LOG(MinimunPWMfrecuency*MotorRevolution,2),0)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
+      <c r="D20" s="8">
+        <f>ROUNDUP(LOG(MinimunPWMfrecuency*MotorRevolution/Mirrors,2),0)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="8">
-        <v>144</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="8">
-        <v>32</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="8">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="8">
         <f>LaserDelay*PWMFrecuency</f>
         <v>144</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="8">
-        <f>MotorRevolution*PWMFrecuency</f>
-        <v>3456000</v>
-      </c>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="8">
+        <f>MotorRevolution/Mirrors*PWMFrecuency</f>
+        <v>1728000</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D27" s="1">
         <f>1/(PWMFrecuency*10^6)*10^12</f>
         <v>6944.4444444444443</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E27" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <f>(UnitInMicroMeters/10^Trailing)*(PrinterTimeLine/PrinterWidth)/(ControllerUnit*10^-6)</f>
         <v>0.54864000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="8"/>
-      <c r="E29" s="13"/>
-    </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30" s="8"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" s="8"/>
-      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" s="8"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1">
+        <v>7980</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>28984</v>
+      </c>
+      <c r="D2">
+        <f>C2-C1</f>
+        <v>21004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>58395</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D20" si="0">C3-C2</f>
+        <v>29411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>64840</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>9077</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-55763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>61497</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>52420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>32678</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-28819</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>13046</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-19632</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>15110</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>46383</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>31273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>43029</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-3354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>19730</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-23299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>20485</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>62612</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>42127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>6274</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-56338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>32367</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>26093</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>60090</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>27723</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>63372</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>46227</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-17145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>5250</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-40977</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>